<commit_message>
updating of bug log for login
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -1,33 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tang Hui Xin\Documents\FYP\metrics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5220769B-2AA2-4DD4-8C19-55A7580EF429}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <fileRecoveryPr autoRecover="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -105,297 +94,791 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>e94ff6c1c40151d7251a2711aeb1074123a5ac87</t>
+  </si>
+  <si>
+    <t>Login (App)</t>
+  </si>
+  <si>
+    <t>The user with the correct email address is unable to login to the app</t>
+  </si>
+  <si>
+    <t>The username was retrieved from the database and validated against the input email address instead</t>
+  </si>
+  <si>
+    <t>17 Jul 2018</t>
+  </si>
+  <si>
+    <t>Hui Xin</t>
+  </si>
+  <si>
+    <t>18 Jul 2018</t>
+  </si>
+  <si>
+    <t>Time taken (h)</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Retrieve the email field from the database instead for validation of email input</t>
+  </si>
+  <si>
+    <t>Error Message was displayed incorrectly</t>
+  </si>
+  <si>
+    <t>Error Message was not displayed incorrectly</t>
+  </si>
+  <si>
+    <t>The error message displayed does not reflect whether the error lies in the password or email</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Correct the error messages displayed</t>
+  </si>
+  <si>
+    <t>Correct the error messages displayed to be more specific</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="31">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="18.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color rgb="FF000000"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3300"/>
-        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="22">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="17" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="18" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="17" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="19" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,10 +887,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,85 +901,85 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,27 +991,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -549,61 +1032,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,26 +1098,98 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="49">
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="29" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="33" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="37" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="41" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="45" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="26" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="30" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="34" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="38" builtinId="43"/>
+    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="46" builtinId="51"/>
+    <cellStyle name="60% - Accent1" xfId="27" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="31" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="35" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="39" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="47" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="24" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="28" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="32" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="36" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="40" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="17" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="18" builtinId="23"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="5" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="6" builtinId="7"/>
+    <cellStyle name="Explanatory Text" xfId="48" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Good" xfId="21" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="11" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="13" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="14" builtinId="19"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="15" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="19" builtinId="24"/>
+    <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Output" xfId="16" builtinId="21"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="Total" xfId="20" builtinId="25"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFFF3300"/>
-    </mruColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -645,41 +1200,41 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>140708</xdr:rowOff>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="table">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{991B2F13-BFC0-459D-B0FB-28D55238C662}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="table" descr="xl/media/image1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="3067049"/>
-          <a:ext cx="4981575" cy="1283709"/>
+          <a:off x="361950" y="6629400"/>
+          <a:ext cx="5695950" cy="1381124"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
+        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -687,43 +1242,43 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>145320</xdr:rowOff>
+      <xdr:rowOff>145415</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="table">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3458B6CE-60A3-4B5E-AADC-4228411A4B44}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="table" descr="xl/media/image2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609599" y="4591050"/>
-          <a:ext cx="4981575" cy="907320"/>
+          <a:off x="285750" y="8229600"/>
+          <a:ext cx="5772150" cy="885825"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
+        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1027,22 +1582,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="A10" zoomScale="126" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.500000"/>
   <cols>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="3" max="3" width="13.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="16.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="17.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" width="18.00499916" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" ht="15.000000" customHeight="1">
       <c r="B3" s="73" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1611,7 @@
       <c r="J3" s="73"/>
       <c r="K3" s="73"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11">
       <c r="B4" s="73"/>
       <c r="C4" s="73"/>
       <c r="D4" s="73"/>
@@ -1068,7 +1623,7 @@
       <c r="J4" s="73"/>
       <c r="K4" s="73"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11">
       <c r="B5" s="73"/>
       <c r="C5" s="73"/>
       <c r="D5" s="73"/>
@@ -1080,7 +1635,7 @@
       <c r="J5" s="73"/>
       <c r="K5" s="73"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11">
       <c r="B6" s="75" t="s">
         <v>1</v>
       </c>
@@ -1106,7 +1661,7 @@
       <c r="J6" s="78"/>
       <c r="K6" s="78"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11">
       <c r="B7" s="79"/>
       <c r="C7" s="78"/>
       <c r="D7" s="77"/>
@@ -1118,7 +1673,7 @@
       <c r="J7" s="78"/>
       <c r="K7" s="78"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="16.500000">
       <c r="B8" s="74">
         <v>1</v>
       </c>
@@ -1144,7 +1699,7 @@
       <c r="J8" s="54"/>
       <c r="K8" s="55"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="16.500000">
       <c r="B9" s="74">
         <v>2</v>
       </c>
@@ -1158,7 +1713,7 @@
       <c r="J9" s="54"/>
       <c r="K9" s="55"/>
     </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" ht="30.000000" customHeight="1">
       <c r="B10" s="74">
         <v>3</v>
       </c>
@@ -1172,7 +1727,7 @@
       <c r="J10" s="57"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" ht="29.250000" customHeight="1">
       <c r="B11" s="74">
         <v>4</v>
       </c>
@@ -1186,7 +1741,7 @@
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="2:11" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="80.250000" customHeight="1">
       <c r="B12" s="74">
         <v>5</v>
       </c>
@@ -1200,7 +1755,7 @@
       <c r="J12" s="54"/>
       <c r="K12" s="55"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" ht="16.500000">
       <c r="B13" s="74">
         <v>6</v>
       </c>
@@ -1214,7 +1769,7 @@
       <c r="J13" s="54"/>
       <c r="K13" s="55"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" ht="16.500000">
       <c r="B14" s="74">
         <v>7</v>
       </c>
@@ -1228,7 +1783,7 @@
       <c r="J14" s="54"/>
       <c r="K14" s="55"/>
     </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" ht="30.000000" customHeight="1">
       <c r="B15" s="74">
         <v>8</v>
       </c>
@@ -1242,7 +1797,7 @@
       <c r="J15" s="57"/>
       <c r="K15" s="58"/>
     </row>
-    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="29.250000" customHeight="1">
       <c r="B16" s="74">
         <v>9</v>
       </c>
@@ -1256,7 +1811,7 @@
       <c r="J16" s="57"/>
       <c r="K16" s="58"/>
     </row>
-    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="29.250000" customHeight="1">
       <c r="B17" s="74">
         <v>10</v>
       </c>
@@ -1270,7 +1825,7 @@
       <c r="J17" s="42"/>
       <c r="K17" s="43"/>
     </row>
-    <row r="18" spans="1:11" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="80.250000" customHeight="1">
       <c r="B18" s="74">
         <v>11</v>
       </c>
@@ -1284,7 +1839,7 @@
       <c r="J18" s="54"/>
       <c r="K18" s="55"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="16.500000">
       <c r="B19" s="74" t="s">
         <v>8</v>
       </c>
@@ -1306,8 +1861,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="16.500000">
       <c r="B21" s="50" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1870,7 @@
       <c r="E21" s="51"/>
       <c r="F21" s="52"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="16.500000">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -1325,7 +1879,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="16.500000">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1334,7 +1888,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="16.500000">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1343,7 +1897,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="16.500000">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1352,7 +1906,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="16.500000">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1363,10 +1917,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B21:F21"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1375,49 +1925,52 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="B21:F21"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.90625000" defaultRowHeight="14.500000" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="17"/>
-    <col min="2" max="2" width="8.90625" style="59"/>
-    <col min="3" max="3" width="20.90625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="17" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="19" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="19" customWidth="1"/>
-    <col min="11" max="12" width="8.90625" style="11"/>
-    <col min="13" max="13" width="13.453125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="11.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.54296875" style="20" customWidth="1"/>
-    <col min="16" max="16" width="24.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.90625" style="11"/>
+    <col min="1" max="1" style="17" width="9.13000011" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" style="59" width="8.88000011" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" style="37" width="20.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" style="11" width="22.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" style="18" width="48.00500107" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" style="11" width="65.12999725" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" style="17" width="13.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" style="19" width="16.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="9" max="10" style="19" width="13.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="11" max="12" style="11" width="8.88000011" customWidth="1" outlineLevel="0"/>
+    <col min="13" max="13" style="19" width="13.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="14" max="14" style="11" width="11.38000011" customWidth="1" outlineLevel="0"/>
+    <col min="15" max="15" style="20" width="25.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="16" max="16384" style="11" width="8.88000011" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="50.800000">
       <c r="A1" s="67" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1999,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K1" s="71" t="s">
         <v>10</v>
@@ -1463,1013 +2016,1017 @@
       <c r="O1" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="10"/>
-    </row>
-    <row r="2" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" ht="45.000000" customHeight="1">
       <c r="A2" s="60">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="13"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B2" s="12">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="45">
+        <v>1</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="26">
+        <v>5</v>
+      </c>
+      <c r="M2" s="31">
+        <v>5</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="34.050000">
       <c r="A3" s="60">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B3" s="12">
+        <v>2</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="12">
+        <v>1</v>
+      </c>
+      <c r="M3" s="31">
+        <v>6</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.500000">
       <c r="A4" s="60">
         <v>3</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="14"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="23"/>
       <c r="H4" s="45"/>
       <c r="I4" s="21"/>
       <c r="J4" s="45"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="45"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="22"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N4" s="82"/>
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="1:16" ht="16.500000">
       <c r="A5" s="60">
         <v>4</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="23"/>
       <c r="H5" s="45"/>
       <c r="I5" s="21"/>
       <c r="J5" s="45"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="45"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="22"/>
-    </row>
-    <row r="6" spans="1:17" s="33" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="82"/>
+      <c r="O5" s="45"/>
+    </row>
+    <row r="6" spans="1:16" s="33" customFormat="1" ht="77.250000" customHeight="1">
       <c r="A6" s="61">
         <v>5</v>
       </c>
       <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="29"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="30"/>
       <c r="H6" s="31"/>
       <c r="I6" s="35"/>
       <c r="J6" s="31"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="31"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="28"/>
-    </row>
-    <row r="7" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="1"/>
+      <c r="O6" s="35"/>
+    </row>
+    <row r="7" spans="1:16" s="33" customFormat="1" ht="14.500000" customHeight="1">
       <c r="A7" s="61">
         <v>6</v>
       </c>
       <c r="B7" s="26"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="32"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="30"/>
       <c r="H7" s="31"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
       <c r="M7" s="31"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="31"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N7" s="1"/>
+      <c r="O7" s="35"/>
+    </row>
+    <row r="8" spans="1:16" ht="16.500000">
       <c r="A8" s="60">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="23"/>
       <c r="H8" s="21"/>
       <c r="I8" s="23"/>
       <c r="J8" s="45"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="45"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="21"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N8" s="82"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.500000">
       <c r="A9" s="60">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="23"/>
       <c r="H9" s="21"/>
       <c r="I9" s="23"/>
       <c r="J9" s="45"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="45"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N9" s="82"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="1:16" ht="16.500000">
       <c r="A10" s="60">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="39"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="23"/>
       <c r="H10" s="21"/>
       <c r="I10" s="23"/>
       <c r="J10" s="45"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="13"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="45"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N10" s="82"/>
+      <c r="O10" s="21"/>
+    </row>
+    <row r="11" spans="1:16" ht="16.500000">
       <c r="A11" s="60">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="36"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
       <c r="G11" s="23"/>
       <c r="H11" s="21"/>
       <c r="I11" s="23"/>
       <c r="J11" s="45"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="13"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="45"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N11" s="82"/>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="1:16" ht="16.500000">
       <c r="A12" s="60">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="84"/>
       <c r="G12" s="23"/>
       <c r="H12" s="21"/>
       <c r="I12" s="23"/>
       <c r="J12" s="45"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="45"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="21"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N12" s="82"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="1:16" ht="17.250000">
       <c r="A13" s="60">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="38"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="87"/>
       <c r="G13" s="23"/>
       <c r="H13" s="21"/>
       <c r="I13" s="23"/>
       <c r="J13" s="45"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="13"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="45"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="21"/>
-    </row>
-    <row r="14" spans="1:17" s="33" customFormat="1" ht="231.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N13" s="82"/>
+      <c r="O13" s="21"/>
+    </row>
+    <row r="14" spans="1:16" s="33" customFormat="1" ht="231.000000" customHeight="1">
       <c r="A14" s="60">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="34"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="88"/>
       <c r="G14" s="30"/>
       <c r="H14" s="35"/>
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="26"/>
       <c r="M14" s="31"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N14" s="82"/>
+      <c r="O14" s="35"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.500000">
       <c r="A15" s="60">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="29"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="30"/>
       <c r="H15" s="35"/>
       <c r="I15" s="30"/>
       <c r="J15" s="45"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="45"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="35"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N15" s="82"/>
+      <c r="O15" s="21"/>
+    </row>
+    <row r="16" spans="1:16" ht="16.500000">
       <c r="A16" s="60">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="30"/>
       <c r="H16" s="35"/>
       <c r="I16" s="30"/>
       <c r="J16" s="45"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="13"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="12"/>
       <c r="M16" s="45"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="35"/>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N16" s="82"/>
+      <c r="O16" s="21"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A17" s="60">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="30"/>
       <c r="H17" s="35"/>
       <c r="I17" s="30"/>
       <c r="J17" s="45"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="13"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="45"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="35"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N17" s="82"/>
+      <c r="O17" s="21"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A18" s="60">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="30"/>
       <c r="H18" s="35"/>
       <c r="I18" s="30"/>
       <c r="J18" s="45"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="13"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="45"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="35"/>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N18" s="82"/>
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A19" s="60">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="24"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="82"/>
       <c r="G19" s="30"/>
       <c r="H19" s="35"/>
       <c r="I19" s="30"/>
       <c r="J19" s="45"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="13"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="12"/>
       <c r="M19" s="45"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="35"/>
-    </row>
-    <row r="20" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N19" s="82"/>
+      <c r="O19" s="21"/>
+    </row>
+    <row r="20" spans="1:15" ht="75.000000" customHeight="1">
       <c r="A20" s="60">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="30"/>
       <c r="H20" s="35"/>
       <c r="I20" s="30"/>
       <c r="J20" s="45"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="13"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="45"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="35"/>
-    </row>
-    <row r="21" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N20" s="82"/>
+      <c r="O20" s="21"/>
+    </row>
+    <row r="21" spans="1:15" ht="75.000000" customHeight="1">
       <c r="A21" s="60">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="30"/>
       <c r="H21" s="35"/>
       <c r="I21" s="30"/>
       <c r="J21" s="45"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="13"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="45"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="35"/>
-    </row>
-    <row r="22" spans="1:16" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N21" s="82"/>
+      <c r="O21" s="21"/>
+    </row>
+    <row r="22" spans="1:15" ht="101.250000" customHeight="1">
       <c r="A22" s="60">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="82"/>
       <c r="G22" s="30"/>
       <c r="H22" s="35"/>
       <c r="I22" s="30"/>
       <c r="J22" s="45"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="13"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="45"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="35"/>
-    </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N22" s="82"/>
+      <c r="O22" s="21"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A23" s="60">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="24"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="82"/>
       <c r="G23" s="30"/>
       <c r="H23" s="35"/>
       <c r="I23" s="30"/>
       <c r="J23" s="45"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="13"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="12"/>
       <c r="M23" s="45"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="35"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N23" s="82"/>
+      <c r="O23" s="21"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A24" s="60">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="24"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="30"/>
       <c r="H24" s="35"/>
       <c r="I24" s="30"/>
       <c r="J24" s="45"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="13"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="12"/>
       <c r="M24" s="45"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="35"/>
-    </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N24" s="82"/>
+      <c r="O24" s="21"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A25" s="60">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="24"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="82"/>
       <c r="G25" s="30"/>
       <c r="H25" s="35"/>
       <c r="I25" s="30"/>
       <c r="J25" s="45"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="13"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="12"/>
       <c r="M25" s="45"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="35"/>
-    </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N25" s="82"/>
+      <c r="O25" s="21"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A26" s="60">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="30"/>
       <c r="H26" s="35"/>
       <c r="I26" s="30"/>
       <c r="J26" s="45"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="13"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="12"/>
       <c r="M26" s="45"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="35"/>
-    </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N26" s="82"/>
+      <c r="O26" s="21"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A27" s="60">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="30"/>
       <c r="H27" s="35"/>
       <c r="I27" s="30"/>
       <c r="J27" s="45"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="13"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="12"/>
       <c r="M27" s="45"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="21"/>
-    </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N27" s="82"/>
+      <c r="O27" s="21"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A28" s="60">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="30"/>
       <c r="H28" s="35"/>
       <c r="I28" s="30"/>
       <c r="J28" s="45"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="13"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="45"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="35"/>
-    </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N28" s="82"/>
+      <c r="O28" s="21"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.000000" customHeight="1">
       <c r="A29" s="60">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="13"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="23"/>
       <c r="H29" s="45"/>
       <c r="I29" s="46"/>
       <c r="J29" s="45"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
       <c r="M29" s="45"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="13"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N29" s="12"/>
+      <c r="O29" s="45"/>
+    </row>
+    <row r="30" spans="1:15" ht="16.500000">
       <c r="A30" s="60">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="13"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="23"/>
       <c r="H30" s="45"/>
       <c r="I30" s="46"/>
       <c r="J30" s="45"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
       <c r="M30" s="45"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N30" s="12"/>
+      <c r="O30" s="45"/>
+    </row>
+    <row r="31" spans="1:15" ht="16.500000">
       <c r="A31" s="60">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="22"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="82"/>
       <c r="G31" s="23"/>
       <c r="H31" s="21"/>
       <c r="I31" s="46"/>
       <c r="J31" s="45"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="13"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="12"/>
       <c r="M31" s="45"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="22"/>
-    </row>
-    <row r="32" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N31" s="82"/>
+      <c r="O31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" ht="30.000000" customHeight="1">
       <c r="A32" s="60">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="22"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="82"/>
       <c r="G32" s="23"/>
       <c r="H32" s="21"/>
       <c r="I32" s="46"/>
       <c r="J32" s="45"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="13"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="12"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="22"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N32" s="82"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" spans="1:15" ht="16.500000">
       <c r="A33" s="60">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="22"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
       <c r="G33" s="23"/>
       <c r="H33" s="21"/>
       <c r="I33" s="46"/>
       <c r="J33" s="45"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="13"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="12"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="22"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N33" s="82"/>
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" spans="1:15" ht="16.500000">
       <c r="A34" s="60">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="22"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
       <c r="G34" s="23"/>
       <c r="H34" s="21"/>
       <c r="I34" s="46"/>
       <c r="J34" s="45"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="13"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="12"/>
       <c r="M34" s="45"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="22"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N34" s="82"/>
+      <c r="O34" s="21"/>
+    </row>
+    <row r="35" spans="1:15" ht="16.500000">
       <c r="A35" s="60">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="82"/>
       <c r="G35" s="23"/>
       <c r="H35" s="21"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="13"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="12"/>
       <c r="M35" s="45"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="22"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N35" s="82"/>
+      <c r="O35" s="21"/>
+    </row>
+    <row r="36" spans="1:15" ht="16.500000">
       <c r="A36" s="60">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="22"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
       <c r="G36" s="23"/>
       <c r="H36" s="21"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="13"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="12"/>
       <c r="M36" s="45"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="22"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N36" s="82"/>
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" spans="1:15" ht="16.500000">
       <c r="A37" s="60">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="22"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
       <c r="G37" s="23"/>
       <c r="H37" s="21"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="13"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="12"/>
       <c r="M37" s="45"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="22"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N37" s="82"/>
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" spans="1:15" ht="16.500000">
       <c r="A38" s="60">
         <v>37</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="22"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="23"/>
       <c r="H38" s="21"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="13"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="12"/>
       <c r="M38" s="45"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="22"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N38" s="82"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" spans="1:15" ht="16.500000">
       <c r="A39" s="60">
         <v>38</v>
       </c>
       <c r="B39" s="12"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="22"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="82"/>
       <c r="G39" s="23"/>
       <c r="H39" s="21"/>
       <c r="I39" s="46"/>
       <c r="J39" s="45"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="13"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="12"/>
       <c r="M39" s="45"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="25"/>
-      <c r="P39" s="22"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N39" s="82"/>
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" spans="1:15" ht="16.500000">
       <c r="A40" s="60">
         <v>39</v>
       </c>
       <c r="B40" s="12"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="22"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="23"/>
       <c r="H40" s="21"/>
       <c r="I40" s="46"/>
       <c r="J40" s="45"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="13"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="12"/>
       <c r="M40" s="45"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="22"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N40" s="82"/>
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" spans="1:15" ht="16.500000">
       <c r="A41" s="60">
         <v>40</v>
       </c>
       <c r="B41" s="12"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="22"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
       <c r="G41" s="23"/>
       <c r="H41" s="21"/>
       <c r="I41" s="46"/>
       <c r="J41" s="45"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="13"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="12"/>
       <c r="M41" s="45"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="22"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N41" s="82"/>
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" spans="1:15" ht="16.500000">
       <c r="A42" s="60">
         <v>41</v>
       </c>
       <c r="B42" s="12"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="22"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
       <c r="G42" s="44"/>
       <c r="H42" s="21"/>
       <c r="I42" s="46"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="13"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="12"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="25"/>
-      <c r="P42" s="22"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N42" s="82"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="1:15" ht="16.500000">
       <c r="A43" s="60">
         <v>42</v>
       </c>
       <c r="B43" s="12"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="22"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
       <c r="G43" s="44"/>
       <c r="H43" s="21"/>
       <c r="I43" s="46"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="13"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="12"/>
       <c r="M43" s="45"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="22"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N43" s="82"/>
+      <c r="O43" s="21"/>
+    </row>
+    <row r="44" spans="1:15" ht="16.500000">
       <c r="A44" s="60">
         <v>43</v>
       </c>
       <c r="B44" s="12"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="22"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="23"/>
       <c r="H44" s="21"/>
       <c r="I44" s="46"/>
       <c r="J44" s="45"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="13"/>
+      <c r="K44" s="82"/>
+      <c r="L44" s="12"/>
       <c r="M44" s="45"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="25"/>
-      <c r="P44" s="22"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N44" s="82"/>
+      <c r="O44" s="21"/>
+    </row>
+    <row r="45" spans="1:15" ht="16.500000">
       <c r="A45" s="60">
         <v>44</v>
       </c>
       <c r="B45" s="12"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="22"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
       <c r="G45" s="23"/>
       <c r="H45" s="21"/>
       <c r="I45" s="46"/>
       <c r="J45" s="45"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="13"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="12"/>
       <c r="M45" s="45"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="22"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N45" s="82"/>
+      <c r="O45" s="21"/>
+    </row>
+    <row r="46" spans="1:15" ht="16.500000">
       <c r="A46" s="60">
         <v>45</v>
       </c>
       <c r="B46" s="12"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="22"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="82"/>
       <c r="G46" s="23"/>
       <c r="H46" s="21"/>
       <c r="I46" s="46"/>
       <c r="J46" s="45"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="13"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="12"/>
       <c r="M46" s="45"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="22"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N46" s="82"/>
+      <c r="O46" s="21"/>
+    </row>
+    <row r="47" spans="1:15" ht="16.500000">
       <c r="A47" s="60">
         <v>46</v>
       </c>
       <c r="B47" s="12"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="22"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="82"/>
       <c r="G47" s="23"/>
       <c r="H47" s="21"/>
       <c r="I47" s="46"/>
       <c r="J47" s="45"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="13"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="12"/>
       <c r="M47" s="45"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="25"/>
-      <c r="P47" s="22"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N47" s="82"/>
+      <c r="O47" s="21"/>
+    </row>
+    <row r="48" spans="1:15" ht="16.500000">
       <c r="A48" s="60">
         <v>47</v>
       </c>
       <c r="B48" s="12"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="22"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="82"/>
       <c r="G48" s="23"/>
       <c r="H48" s="21"/>
       <c r="I48" s="46"/>
       <c r="J48" s="45"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="13"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="12"/>
       <c r="M48" s="45"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="25"/>
-      <c r="P48" s="22"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N48" s="82"/>
+      <c r="O48" s="21"/>
+    </row>
+    <row r="49" spans="1:15" ht="16.500000">
       <c r="A49" s="60">
         <v>48</v>
       </c>
       <c r="B49" s="12"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="24"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="92"/>
+      <c r="F49" s="82"/>
       <c r="G49" s="23"/>
       <c r="H49" s="21"/>
       <c r="I49" s="46"/>
       <c r="J49" s="45"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="13"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="12"/>
       <c r="M49" s="45"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="22"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N49" s="82"/>
+      <c r="O49" s="21"/>
+    </row>
+    <row r="50" spans="1:15" ht="16.500000">
       <c r="A50" s="60">
         <v>49</v>
       </c>
       <c r="B50" s="12"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="22"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
       <c r="G50" s="23"/>
       <c r="H50" s="21"/>
       <c r="I50" s="46"/>
       <c r="J50" s="45"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="13"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="12"/>
       <c r="M50" s="45"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="25"/>
-      <c r="P50" s="22"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N50" s="82"/>
+      <c r="O50" s="21"/>
+    </row>
+    <row r="51" spans="1:15" ht="16.500000">
       <c r="A51" s="60">
         <v>50</v>
       </c>
       <c r="B51" s="12"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="92"/>
+      <c r="F51" s="93"/>
       <c r="G51" s="23"/>
       <c r="H51" s="21"/>
       <c r="I51" s="46"/>
       <c r="J51" s="45"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
       <c r="M51" s="45"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="25"/>
-      <c r="P51" s="22"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bugs for Creating a tutor after validation
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYU\Documents\YR3 Term1\IS Application Project\Thriving-Stones-Project\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\y3s1\IS480 FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9912579-9D02-4E94-AFCA-FC73C0AF4C63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="36" windowWidth="25752" windowHeight="11592" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -164,58 +165,47 @@
   </si>
   <si>
     <t>There is no validation for student data inputs (StudentID, Phone number, age, gender, reqAmt, etc)</t>
+  </si>
+  <si>
+    <t>Create Tutor (Web)</t>
+  </si>
+  <si>
+    <t>Tutor created is not reflected in the database</t>
+  </si>
+  <si>
+    <t>Wrong method used to store objects in database (SetValueAsync instead of SetValue)</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>Changed to method used in TutorDAO.</t>
+  </si>
+  <si>
+    <t>21094817ecc3a115a2307add56ff0c9213551fdd</t>
+  </si>
+  <si>
+    <t>Tutor created is not reflected in the database (after adding in validation)</t>
+  </si>
+  <si>
+    <t>8a7136c020a39d26976638658563e64f16ac38b3</t>
+  </si>
+  <si>
+    <t>Errors in regex that caused validation error</t>
+  </si>
+  <si>
+    <t>Resolved regex error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,17 +215,74 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -243,17 +290,20 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -275,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -403,17 +453,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -435,12 +474,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,10 +529,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,18 +543,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -483,10 +563,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -504,58 +584,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -564,35 +626,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -612,26 +689,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1056,98 +1157,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K27"/>
   <sheetViews>
     <sheetView zoomScale="126" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="61" t="s">
+    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="62" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="66" t="s">
+      <c r="G6" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="63"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="49"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="33">
         <v>1</v>
       </c>
@@ -1166,14 +1267,14 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="56"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="33">
         <v>2</v>
       </c>
@@ -1182,12 +1283,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="57"/>
-    </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="56"/>
+    </row>
+    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="33">
         <v>3</v>
       </c>
@@ -1196,12 +1297,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="60"/>
-    </row>
-    <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
+    </row>
+    <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="33">
         <v>4</v>
       </c>
@@ -1210,12 +1311,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60"/>
-    </row>
-    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
+    </row>
+    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33">
         <v>5</v>
       </c>
@@ -1224,12 +1325,12 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="57"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H12" s="57"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="33">
         <v>6</v>
       </c>
@@ -1238,12 +1339,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="57"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="33">
         <v>7</v>
       </c>
@@ -1252,12 +1353,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="57"/>
-    </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="54"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="33">
         <v>8</v>
       </c>
@@ -1266,12 +1367,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-    </row>
-    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
+    </row>
+    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="33">
         <v>9</v>
       </c>
@@ -1280,12 +1381,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="60"/>
-    </row>
-    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="59"/>
+    </row>
+    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="33">
         <v>10</v>
       </c>
@@ -1299,7 +1400,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="33">
         <v>11</v>
       </c>
@@ -1308,12 +1409,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="57"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="57"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="56"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="33" t="s">
         <v>8</v>
       </c>
@@ -1335,16 +1436,16 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="54"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -1353,7 +1454,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1362,7 +1463,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1371,7 +1472,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1380,7 +1481,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1391,6 +1492,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1399,19 +1511,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1419,33 +1520,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="11" customWidth="1"/>
     <col min="5" max="5" width="48" style="13" customWidth="1"/>
-    <col min="6" max="6" width="65.109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="14" customWidth="1"/>
-    <col min="9" max="10" width="13.5546875" style="14" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="25.5546875" style="15" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="65.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="14" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" style="14" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="14" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" style="15" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
@@ -1493,8 +1594,8 @@
       </c>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45">
+    <row r="2" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39">
         <v>1</v>
       </c>
       <c r="B2" s="18">
@@ -1512,7 +1613,7 @@
       <c r="F2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="65" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="18" t="s">
@@ -1540,8 +1641,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="45">
+    <row r="3" spans="1:16" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="39">
         <v>2</v>
       </c>
       <c r="B3" s="18">
@@ -1559,7 +1660,7 @@
       <c r="F3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="65" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1587,55 +1688,55 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="19" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45">
+    <row r="4" spans="1:16" s="19" customFormat="1" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39">
         <v>3</v>
       </c>
       <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="44" t="s">
-        <v>37</v>
+      <c r="C4" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="64" t="s">
+        <v>32</v>
       </c>
       <c r="L4" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M4" s="18">
-        <v>7</v>
-      </c>
-      <c r="N4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="48" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="45">
+      <c r="O4" s="64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="39">
         <v>4</v>
       </c>
       <c r="B5" s="18">
@@ -1644,32 +1745,32 @@
       <c r="C5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="38" t="s">
         <v>42</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>30</v>
       </c>
       <c r="J5" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="K5" s="44" t="s">
-        <v>32</v>
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="L5" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M5" s="18">
         <v>12</v>
@@ -1677,79 +1778,135 @@
       <c r="N5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="19" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="18">
+        <v>5</v>
+      </c>
+      <c r="M6" s="18">
+        <v>17</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="64" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="19" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45">
+    <row r="7" spans="1:16" s="19" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="66">
+        <v>43300</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="66">
+        <v>43300</v>
+      </c>
+      <c r="J7" s="18">
+        <v>1</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-    </row>
-    <row r="7" spans="1:16" s="19" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="49">
+      <c r="M7" s="18">
+        <v>22</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
         <v>7</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="34"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-    </row>
-    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
+      <c r="D8" s="38"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="64"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
         <v>8</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="20"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="50"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="50"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="25"/>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
@@ -1757,18 +1914,18 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="49">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
         <v>9</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="20"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="50"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="50"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="25"/>
       <c r="K10" s="16"/>
       <c r="L10" s="25"/>
@@ -1776,18 +1933,18 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="49">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="43">
         <v>10</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="34"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="50"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="50"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="25"/>
       <c r="K11" s="16"/>
       <c r="L11" s="25"/>
@@ -1795,18 +1952,18 @@
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="49">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
         <v>11</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="20"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="50"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="50"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="25"/>
       <c r="K12" s="16"/>
       <c r="L12" s="25"/>
@@ -1814,18 +1971,18 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="49">
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="43">
         <v>12</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="20"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="50"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="69"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="50"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="25"/>
       <c r="K13" s="16"/>
       <c r="L13" s="25"/>
@@ -1833,18 +1990,18 @@
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
     </row>
-    <row r="14" spans="1:16" s="19" customFormat="1" ht="231" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49">
+    <row r="14" spans="1:16" s="19" customFormat="1" ht="231" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
         <v>13</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="47"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="18"/>
       <c r="K14" s="20"/>
       <c r="L14" s="18"/>
@@ -1852,18 +2009,18 @@
       <c r="N14" s="16"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
         <v>14</v>
       </c>
       <c r="B15" s="25"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="16"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="47"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="47"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="25"/>
       <c r="K15" s="20"/>
       <c r="L15" s="25"/>
@@ -1871,18 +2028,18 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="49">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
         <v>15</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="42"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="47"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="47"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="25"/>
       <c r="K16" s="16"/>
       <c r="L16" s="25"/>
@@ -1890,8 +2047,8 @@
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43">
         <v>16</v>
       </c>
       <c r="B17" s="25"/>
@@ -1899,9 +2056,9 @@
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="47"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="47"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="25"/>
       <c r="K17" s="16"/>
       <c r="L17" s="25"/>
@@ -1909,8 +2066,8 @@
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
         <v>17</v>
       </c>
       <c r="B18" s="25"/>
@@ -1918,9 +2075,9 @@
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="47"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="25"/>
       <c r="K18" s="16"/>
       <c r="L18" s="25"/>
@@ -1928,8 +2085,8 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
         <v>18</v>
       </c>
       <c r="B19" s="25"/>
@@ -1937,9 +2094,9 @@
       <c r="D19" s="18"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="47"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="47"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="25"/>
       <c r="K19" s="16"/>
       <c r="L19" s="25"/>
@@ -1947,8 +2104,8 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49">
+    <row r="20" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43">
         <v>19</v>
       </c>
       <c r="B20" s="25"/>
@@ -1956,9 +2113,9 @@
       <c r="D20" s="18"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="47"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="47"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="25"/>
       <c r="K20" s="16"/>
       <c r="L20" s="25"/>
@@ -1966,8 +2123,8 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49">
+    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
         <v>20</v>
       </c>
       <c r="B21" s="25"/>
@@ -1975,9 +2132,9 @@
       <c r="D21" s="20"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="47"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="47"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="25"/>
       <c r="K21" s="16"/>
       <c r="L21" s="25"/>
@@ -1985,8 +2142,8 @@
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
     </row>
-    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49">
+    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
         <v>21</v>
       </c>
       <c r="B22" s="25"/>
@@ -1994,9 +2151,9 @@
       <c r="D22" s="20"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="47"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="47"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="25"/>
       <c r="K22" s="16"/>
       <c r="L22" s="25"/>
@@ -2004,8 +2161,8 @@
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43">
         <v>22</v>
       </c>
       <c r="B23" s="25"/>
@@ -2013,9 +2170,9 @@
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="47"/>
+      <c r="G23" s="41"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="47"/>
+      <c r="I23" s="41"/>
       <c r="J23" s="25"/>
       <c r="K23" s="16"/>
       <c r="L23" s="25"/>
@@ -2023,8 +2180,8 @@
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="43">
         <v>23</v>
       </c>
       <c r="B24" s="25"/>
@@ -2032,9 +2189,9 @@
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="47"/>
+      <c r="G24" s="41"/>
       <c r="H24" s="20"/>
-      <c r="I24" s="47"/>
+      <c r="I24" s="41"/>
       <c r="J24" s="25"/>
       <c r="K24" s="16"/>
       <c r="L24" s="25"/>
@@ -2042,8 +2199,8 @@
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43">
         <v>24</v>
       </c>
       <c r="B25" s="25"/>
@@ -2051,9 +2208,9 @@
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="47"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="47"/>
+      <c r="I25" s="41"/>
       <c r="J25" s="25"/>
       <c r="K25" s="16"/>
       <c r="L25" s="25"/>
@@ -2061,8 +2218,8 @@
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="43">
         <v>25</v>
       </c>
       <c r="B26" s="25"/>
@@ -2070,9 +2227,9 @@
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="47"/>
+      <c r="G26" s="41"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="47"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="25"/>
       <c r="K26" s="16"/>
       <c r="L26" s="25"/>
@@ -2080,8 +2237,8 @@
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43">
         <v>26</v>
       </c>
       <c r="B27" s="25"/>
@@ -2089,9 +2246,9 @@
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="47"/>
+      <c r="G27" s="41"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="47"/>
+      <c r="I27" s="41"/>
       <c r="J27" s="25"/>
       <c r="K27" s="16"/>
       <c r="L27" s="25"/>
@@ -2099,8 +2256,8 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="49">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="43">
         <v>27</v>
       </c>
       <c r="B28" s="25"/>
@@ -2108,9 +2265,9 @@
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="47"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="47"/>
+      <c r="I28" s="41"/>
       <c r="J28" s="25"/>
       <c r="K28" s="16"/>
       <c r="L28" s="25"/>
@@ -2118,8 +2275,8 @@
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="49">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43">
         <v>28</v>
       </c>
       <c r="B29" s="25"/>
@@ -2127,7 +2284,7 @@
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="50"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="25"/>
       <c r="I29" s="26"/>
       <c r="J29" s="25"/>
@@ -2137,8 +2294,8 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
     </row>
-    <row r="30" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="49">
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="43">
         <v>29</v>
       </c>
       <c r="B30" s="25"/>
@@ -2146,7 +2303,7 @@
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
-      <c r="G30" s="50"/>
+      <c r="G30" s="44"/>
       <c r="H30" s="25"/>
       <c r="I30" s="26"/>
       <c r="J30" s="25"/>
@@ -2156,8 +2313,8 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="49">
+    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="43">
         <v>30</v>
       </c>
       <c r="B31" s="25"/>
@@ -2165,7 +2322,7 @@
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="16"/>
       <c r="I31" s="26"/>
       <c r="J31" s="25"/>
@@ -2175,8 +2332,8 @@
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="49">
+    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43">
         <v>31</v>
       </c>
       <c r="B32" s="25"/>
@@ -2184,7 +2341,7 @@
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="50"/>
+      <c r="G32" s="44"/>
       <c r="H32" s="16"/>
       <c r="I32" s="26"/>
       <c r="J32" s="25"/>
@@ -2194,8 +2351,8 @@
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
     </row>
-    <row r="33" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="49">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="43">
         <v>32</v>
       </c>
       <c r="B33" s="25"/>
@@ -2203,7 +2360,7 @@
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="50"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="16"/>
       <c r="I33" s="26"/>
       <c r="J33" s="25"/>
@@ -2213,8 +2370,8 @@
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="49">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="43">
         <v>33</v>
       </c>
       <c r="B34" s="25"/>
@@ -2222,7 +2379,7 @@
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="50"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="16"/>
       <c r="I34" s="26"/>
       <c r="J34" s="25"/>
@@ -2232,8 +2389,8 @@
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
     </row>
-    <row r="35" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="49">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="43">
         <v>34</v>
       </c>
       <c r="B35" s="25"/>
@@ -2241,7 +2398,7 @@
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="50"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="16"/>
       <c r="I35" s="26"/>
       <c r="J35" s="25"/>
@@ -2251,8 +2408,8 @@
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
     </row>
-    <row r="36" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="49">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="43">
         <v>35</v>
       </c>
       <c r="B36" s="25"/>
@@ -2260,7 +2417,7 @@
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="50"/>
+      <c r="G36" s="44"/>
       <c r="H36" s="16"/>
       <c r="I36" s="25"/>
       <c r="J36" s="25"/>
@@ -2270,8 +2427,8 @@
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="49">
+    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="43">
         <v>36</v>
       </c>
       <c r="B37" s="25"/>
@@ -2279,7 +2436,7 @@
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="50"/>
+      <c r="G37" s="44"/>
       <c r="H37" s="16"/>
       <c r="I37" s="26"/>
       <c r="J37" s="25"/>
@@ -2289,8 +2446,8 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
     </row>
-    <row r="38" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="49">
+    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="43">
         <v>37</v>
       </c>
       <c r="B38" s="25"/>
@@ -2298,7 +2455,7 @@
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="50"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="16"/>
       <c r="I38" s="25"/>
       <c r="J38" s="25"/>
@@ -2308,8 +2465,8 @@
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
     </row>
-    <row r="39" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="49">
+    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="43">
         <v>38</v>
       </c>
       <c r="B39" s="25"/>
@@ -2317,7 +2474,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="50"/>
+      <c r="G39" s="44"/>
       <c r="H39" s="16"/>
       <c r="I39" s="26"/>
       <c r="J39" s="25"/>
@@ -2327,8 +2484,8 @@
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
     </row>
-    <row r="40" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="49">
+    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="43">
         <v>39</v>
       </c>
       <c r="B40" s="25"/>
@@ -2336,7 +2493,7 @@
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="50"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="16"/>
       <c r="I40" s="26"/>
       <c r="J40" s="25"/>
@@ -2346,8 +2503,8 @@
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
     </row>
-    <row r="41" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="49">
+    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="43">
         <v>40</v>
       </c>
       <c r="B41" s="25"/>
@@ -2355,7 +2512,7 @@
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="50"/>
+      <c r="G41" s="44"/>
       <c r="H41" s="16"/>
       <c r="I41" s="26"/>
       <c r="J41" s="25"/>
@@ -2365,8 +2522,8 @@
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
     </row>
-    <row r="42" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="49">
+    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="43">
         <v>41</v>
       </c>
       <c r="B42" s="25"/>
@@ -2384,8 +2541,8 @@
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
     </row>
-    <row r="43" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="49">
+    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="43">
         <v>42</v>
       </c>
       <c r="B43" s="25"/>
@@ -2403,8 +2560,8 @@
       <c r="N43" s="16"/>
       <c r="O43" s="16"/>
     </row>
-    <row r="44" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="49">
+    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="43">
         <v>43</v>
       </c>
       <c r="B44" s="25"/>
@@ -2412,7 +2569,7 @@
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="50"/>
+      <c r="G44" s="44"/>
       <c r="H44" s="16"/>
       <c r="I44" s="26"/>
       <c r="J44" s="25"/>
@@ -2422,8 +2579,8 @@
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="49">
+    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="43">
         <v>44</v>
       </c>
       <c r="B45" s="25"/>
@@ -2431,7 +2588,7 @@
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="50"/>
+      <c r="G45" s="44"/>
       <c r="H45" s="16"/>
       <c r="I45" s="26"/>
       <c r="J45" s="25"/>
@@ -2441,8 +2598,8 @@
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="49">
+    <row r="46" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="43">
         <v>45</v>
       </c>
       <c r="B46" s="25"/>
@@ -2450,7 +2607,7 @@
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="50"/>
+      <c r="G46" s="44"/>
       <c r="H46" s="16"/>
       <c r="I46" s="26"/>
       <c r="J46" s="25"/>
@@ -2460,8 +2617,8 @@
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="49">
+    <row r="47" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="43">
         <v>46</v>
       </c>
       <c r="B47" s="25"/>
@@ -2469,7 +2626,7 @@
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
-      <c r="G47" s="50"/>
+      <c r="G47" s="44"/>
       <c r="H47" s="16"/>
       <c r="I47" s="26"/>
       <c r="J47" s="25"/>
@@ -2479,16 +2636,16 @@
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
     </row>
-    <row r="48" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="49">
+    <row r="48" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="43">
         <v>47</v>
       </c>
       <c r="B48" s="25"/>
-      <c r="C48" s="51"/>
+      <c r="C48" s="45"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="50"/>
+      <c r="G48" s="44"/>
       <c r="H48" s="16"/>
       <c r="I48" s="26"/>
       <c r="J48" s="25"/>
@@ -2498,16 +2655,16 @@
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
     </row>
-    <row r="49" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="49">
+    <row r="49" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="43">
         <v>48</v>
       </c>
       <c r="B49" s="25"/>
       <c r="C49" s="20"/>
       <c r="D49" s="16"/>
-      <c r="E49" s="43"/>
+      <c r="E49" s="37"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="50"/>
+      <c r="G49" s="44"/>
       <c r="H49" s="16"/>
       <c r="I49" s="26"/>
       <c r="J49" s="25"/>
@@ -2517,8 +2674,8 @@
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
     </row>
-    <row r="50" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="49">
+    <row r="50" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="43">
         <v>49</v>
       </c>
       <c r="B50" s="25"/>
@@ -2526,7 +2683,7 @@
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="50"/>
+      <c r="G50" s="44"/>
       <c r="H50" s="16"/>
       <c r="I50" s="26"/>
       <c r="J50" s="25"/>
@@ -2536,27 +2693,27 @@
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
     </row>
-    <row r="51" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="49">
+    <row r="51" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="43">
         <v>50</v>
       </c>
       <c r="B51" s="25"/>
       <c r="C51" s="20"/>
       <c r="D51" s="16"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="50"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="44"/>
       <c r="H51" s="16"/>
       <c r="I51" s="26"/>
       <c r="J51" s="25"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
       <c r="M51" s="25"/>
-      <c r="N51" s="43"/>
+      <c r="N51" s="37"/>
       <c r="O51" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
updating of bug and task metrics
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\y3s1\IS480 FYP\Thriving-Stones-Project\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tang Hui Xin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9912579-9D02-4E94-AFCA-FC73C0AF4C63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E88E2C-EB61-4053-A5E0-5ED900BD80B3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Resolved regex error</t>
+  </si>
+  <si>
+    <t>As the bugs were found during the testing sessions, we fixed it during the designated bug fixing sessions before proceeding on with the other tasks</t>
   </si>
 </sst>
 </file>
@@ -204,11 +207,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -518,9 +528,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,10 +539,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,18 +553,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -563,10 +573,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -584,40 +594,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,112 +636,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,7 +836,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>145415</xdr:rowOff>
+      <xdr:rowOff>145416</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1160,95 +1179,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K27"/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="126" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="70"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="33">
         <v>1</v>
       </c>
@@ -1267,28 +1286,40 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="64"/>
+    </row>
+    <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33">
         <v>2</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
-    </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>22</v>
+      </c>
+      <c r="H9" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="77"/>
+    </row>
+    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="33">
         <v>3</v>
       </c>
@@ -1297,12 +1328,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="59"/>
-    </row>
-    <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67"/>
+    </row>
+    <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="33">
         <v>4</v>
       </c>
@@ -1311,12 +1342,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-    </row>
-    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="65"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="67"/>
+    </row>
+    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="33">
         <v>5</v>
       </c>
@@ -1325,12 +1356,12 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="65"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="64"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="33">
         <v>6</v>
       </c>
@@ -1339,12 +1370,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H13" s="62"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="33">
         <v>7</v>
       </c>
@@ -1353,12 +1384,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
-    </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="33">
         <v>8</v>
       </c>
@@ -1367,12 +1398,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="59"/>
-    </row>
-    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="67"/>
+    </row>
+    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="33">
         <v>9</v>
       </c>
@@ -1381,12 +1412,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="59"/>
-    </row>
-    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="67"/>
+    </row>
+    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="33">
         <v>10</v>
       </c>
@@ -1400,7 +1431,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="33">
         <v>11</v>
       </c>
@@ -1409,12 +1440,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="65"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="64"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
         <v>8</v>
       </c>
@@ -1436,16 +1467,16 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="60" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B21" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="62"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="61"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -1454,7 +1485,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1463,7 +1494,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1472,7 +1503,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1481,7 +1512,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1492,17 +1523,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1511,8 +1531,19 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1523,30 +1554,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" style="11" customWidth="1"/>
     <col min="5" max="5" width="48" style="13" customWidth="1"/>
-    <col min="6" max="6" width="65.140625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="14" customWidth="1"/>
-    <col min="9" max="10" width="13.5703125" style="14" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" style="15" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="11"/>
+    <col min="6" max="6" width="65.1796875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="14" customWidth="1"/>
+    <col min="9" max="10" width="13.54296875" style="14" customWidth="1"/>
+    <col min="11" max="12" width="8.81640625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="11.26953125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="25.54296875" style="15" customWidth="1"/>
+    <col min="16" max="16" width="8.81640625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.81640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
@@ -1594,7 +1625,7 @@
       </c>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -1613,7 +1644,7 @@
       <c r="F2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="49" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="18" t="s">
@@ -1641,7 +1672,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="19" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -1660,7 +1691,7 @@
       <c r="F3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="49" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1688,38 +1719,38 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="19" customFormat="1" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="19" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="39">
         <v>3</v>
       </c>
       <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="48" t="s">
         <v>51</v>
       </c>
       <c r="I4" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="64">
+      <c r="J4" s="48">
         <v>0.5</v>
       </c>
-      <c r="K4" s="64" t="s">
+      <c r="K4" s="48" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="18">
@@ -1728,14 +1759,14 @@
       <c r="M4" s="18">
         <v>11</v>
       </c>
-      <c r="N4" s="64" t="s">
+      <c r="N4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="64" t="s">
+      <c r="O4" s="48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="42" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -1754,7 +1785,7 @@
       <c r="F5" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="49" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="38" t="s">
@@ -1782,7 +1813,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="19" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="19" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -1801,7 +1832,7 @@
       <c r="F6" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="49" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="38" t="s">
@@ -1825,11 +1856,11 @@
       <c r="N6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="64" t="s">
+      <c r="O6" s="48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="19" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="19" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="39">
         <v>6</v>
       </c>
@@ -1839,22 +1870,22 @@
       <c r="C7" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="48" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="50">
         <v>43300</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="66">
+      <c r="I7" s="50">
         <v>43300</v>
       </c>
       <c r="J7" s="18">
@@ -1876,7 +1907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>7</v>
       </c>
@@ -1884,7 +1915,7 @@
       <c r="C8" s="34"/>
       <c r="D8" s="38"/>
       <c r="E8" s="40"/>
-      <c r="F8" s="70"/>
+      <c r="F8" s="54"/>
       <c r="G8" s="18"/>
       <c r="H8" s="38"/>
       <c r="I8" s="18"/>
@@ -1893,18 +1924,18 @@
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="20"/>
-      <c r="O8" s="64"/>
-    </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="O8" s="48"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>8</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="20"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="69"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="53"/>
       <c r="H9" s="16"/>
       <c r="I9" s="44"/>
       <c r="J9" s="25"/>
@@ -1914,7 +1945,7 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>9</v>
       </c>
@@ -1922,8 +1953,8 @@
       <c r="C10" s="20"/>
       <c r="D10" s="16"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="69"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="16"/>
       <c r="I10" s="44"/>
       <c r="J10" s="25"/>
@@ -1933,16 +1964,16 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>10</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="34"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="69"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="16"/>
       <c r="I11" s="44"/>
       <c r="J11" s="25"/>
@@ -1952,16 +1983,16 @@
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>11</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="20"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="69"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="16"/>
       <c r="I12" s="44"/>
       <c r="J12" s="25"/>
@@ -1971,16 +2002,16 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="43">
         <v>12</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="20"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="69"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="16"/>
       <c r="I13" s="44"/>
       <c r="J13" s="25"/>
@@ -1990,7 +2021,7 @@
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
     </row>
-    <row r="14" spans="1:16" s="19" customFormat="1" ht="231" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="19" customFormat="1" ht="231" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43">
         <v>13</v>
       </c>
@@ -1998,7 +2029,7 @@
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="71"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="41"/>
       <c r="H14" s="20"/>
       <c r="I14" s="41"/>
@@ -2009,7 +2040,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="43">
         <v>14</v>
       </c>
@@ -2028,7 +2059,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="43">
         <v>15</v>
       </c>
@@ -2047,7 +2078,7 @@
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>16</v>
       </c>
@@ -2066,7 +2097,7 @@
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>17</v>
       </c>
@@ -2085,7 +2116,7 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43">
         <v>18</v>
       </c>
@@ -2104,7 +2135,7 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="43">
         <v>19</v>
       </c>
@@ -2123,7 +2154,7 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="43">
         <v>20</v>
       </c>
@@ -2142,7 +2173,7 @@
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
     </row>
-    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="43">
         <v>21</v>
       </c>
@@ -2161,7 +2192,7 @@
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="43">
         <v>22</v>
       </c>
@@ -2180,7 +2211,7 @@
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="43">
         <v>23</v>
       </c>
@@ -2199,7 +2230,7 @@
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>24</v>
       </c>
@@ -2218,7 +2249,7 @@
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="43">
         <v>25</v>
       </c>
@@ -2237,7 +2268,7 @@
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="43">
         <v>26</v>
       </c>
@@ -2256,7 +2287,7 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="43">
         <v>27</v>
       </c>
@@ -2275,7 +2306,7 @@
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="43">
         <v>28</v>
       </c>
@@ -2294,7 +2325,7 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
     </row>
-    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="43">
         <v>29</v>
       </c>
@@ -2313,7 +2344,7 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="43">
         <v>30</v>
       </c>
@@ -2332,7 +2363,7 @@
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="43">
         <v>31</v>
       </c>
@@ -2351,7 +2382,7 @@
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
     </row>
-    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="43">
         <v>32</v>
       </c>
@@ -2370,7 +2401,7 @@
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="43">
         <v>33</v>
       </c>
@@ -2389,7 +2420,7 @@
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
     </row>
-    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="43">
         <v>34</v>
       </c>
@@ -2408,7 +2439,7 @@
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
     </row>
-    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="43">
         <v>35</v>
       </c>
@@ -2427,7 +2458,7 @@
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="43">
         <v>36</v>
       </c>
@@ -2446,7 +2477,7 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
     </row>
-    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="43">
         <v>37</v>
       </c>
@@ -2465,7 +2496,7 @@
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
     </row>
-    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="43">
         <v>38</v>
       </c>
@@ -2484,7 +2515,7 @@
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
     </row>
-    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="43">
         <v>39</v>
       </c>
@@ -2503,7 +2534,7 @@
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
     </row>
-    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="43">
         <v>40</v>
       </c>
@@ -2522,7 +2553,7 @@
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="43">
         <v>41</v>
       </c>
@@ -2541,7 +2572,7 @@
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
     </row>
-    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="43">
         <v>42</v>
       </c>
@@ -2560,7 +2591,7 @@
       <c r="N43" s="16"/>
       <c r="O43" s="16"/>
     </row>
-    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43">
         <v>43</v>
       </c>
@@ -2579,7 +2610,7 @@
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="43">
         <v>44</v>
       </c>
@@ -2598,7 +2629,7 @@
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="43">
         <v>45</v>
       </c>
@@ -2617,7 +2648,7 @@
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="43">
         <v>46</v>
       </c>
@@ -2636,7 +2667,7 @@
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
     </row>
-    <row r="48" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="43">
         <v>47</v>
       </c>
@@ -2655,7 +2686,7 @@
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
     </row>
-    <row r="49" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="43">
         <v>48</v>
       </c>
@@ -2674,7 +2705,7 @@
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
     </row>
-    <row r="50" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="43">
         <v>49</v>
       </c>
@@ -2693,7 +2724,7 @@
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
     </row>
-    <row r="51" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="43">
         <v>50</v>
       </c>
@@ -2713,7 +2744,7 @@
       <c r="O51" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
logging of bug for reset password
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tang Hui Xin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuiXin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E88E2C-EB61-4053-A5E0-5ED900BD80B3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CAA265-71E1-4B70-AE90-B8C61F476CA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>As the bugs were found during the testing sessions, we fixed it during the designated bug fixing sessions before proceeding on with the other tasks</t>
+  </si>
+  <si>
+    <t>a1171e265566f2979ce323ba65d73b4ea24b24a2</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>Unable to retrieve the correct user from the database</t>
+  </si>
+  <si>
+    <t>Error in the retrieval method for tutors</t>
+  </si>
+  <si>
+    <t>Zang Yu</t>
+  </si>
+  <si>
+    <t>Corrected the retrieval method by modifying the query</t>
   </si>
 </sst>
 </file>
@@ -207,11 +225,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -528,9 +553,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -539,10 +564,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -553,18 +578,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -573,10 +598,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -594,40 +619,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,25 +661,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -663,22 +688,22 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,20 +715,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,6 +751,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -723,34 +769,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1179,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="126" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="126" workbookViewId="0">
       <selection activeCell="H10" sqref="H10:K10"/>
     </sheetView>
   </sheetViews>
@@ -1192,80 +1220,80 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="71" t="s">
+      <c r="H6" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="70"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="33">
@@ -1286,12 +1314,12 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="62" t="s">
+      <c r="H8" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="64"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
     </row>
     <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33">
@@ -1312,12 +1340,12 @@
       <c r="G9" s="1">
         <v>22</v>
       </c>
-      <c r="H9" s="75" t="s">
+      <c r="H9" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="77"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
     </row>
     <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="33">
@@ -1328,10 +1356,10 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="74"/>
     </row>
     <row r="11" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="33">
@@ -1342,10 +1370,10 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="67"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="74"/>
     </row>
     <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="33">
@@ -1356,10 +1384,10 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="33">
@@ -1370,10 +1398,10 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="33">
@@ -1384,10 +1412,10 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="68"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="33">
@@ -1398,10 +1426,10 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="74"/>
     </row>
     <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="33">
@@ -1412,10 +1440,10 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="67"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="74"/>
     </row>
     <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="33">
@@ -1440,10 +1468,10 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="64"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
@@ -1468,13 +1496,13 @@
       <c r="G19" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -1523,6 +1551,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1531,19 +1570,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1554,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="F2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1907,24 +1935,52 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>7</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="48"/>
+      <c r="B8" s="25">
+        <v>3</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="50">
+        <v>43341</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="50">
+        <v>43314</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="18">
+        <v>5</v>
+      </c>
+      <c r="M8" s="18">
+        <v>5</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="78" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
@@ -2744,7 +2800,7 @@
       <c r="O51" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
updating of metrics for iter 5
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369CE3CE-ED96-44FF-9646-385168D93969}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37401DF-CCB8-4837-8BF9-5CC8C71656BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="102">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -278,16 +278,55 @@
     <t>The error message is not displayed when grade update is unsuccessful</t>
   </si>
   <si>
-    <t>16/08/2019</t>
-  </si>
-  <si>
     <t>Missing validation</t>
   </si>
   <si>
-    <t>16/08/2020</t>
-  </si>
-  <si>
     <t>The bugs were fixed during the designated bug fixing sessions</t>
+  </si>
+  <si>
+    <t>123d5e72a28deadf1651bc472a7a5fd03c954537</t>
+  </si>
+  <si>
+    <t>19/08/2018</t>
+  </si>
+  <si>
+    <t>Added error message in front end</t>
+  </si>
+  <si>
+    <t>Attendance Taking</t>
+  </si>
+  <si>
+    <t>When attendance is marked, the checkbox doesn’t disappear and users are confused</t>
+  </si>
+  <si>
+    <t>Poor Interface Design</t>
+  </si>
+  <si>
+    <t>31/08/2018</t>
+  </si>
+  <si>
+    <t>Manage Acc</t>
+  </si>
+  <si>
+    <t>Crashes when accessing page</t>
+  </si>
+  <si>
+    <t>Did not change the method name when we renamed it in the DAO</t>
+  </si>
+  <si>
+    <t>31/08/2019</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Changed the method name accordingly</t>
+  </si>
+  <si>
+    <t>669ddc1f9a6e3d8c79a4a2a85ba046489fe0d000</t>
+  </si>
+  <si>
+    <t>The bugs were discovered during the testing of the functionalities and hence we fixed it immediately upon discovery</t>
   </si>
 </sst>
 </file>
@@ -297,11 +336,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -653,9 +699,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -664,10 +710,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -678,18 +724,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -698,10 +744,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -719,40 +765,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,25 +807,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -788,22 +834,22 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -815,59 +861,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -875,38 +954,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1335,7 +1399,7 @@
   <dimension ref="A3:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="126" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H12" sqref="H12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1347,80 +1411,80 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="85" t="s">
+      <c r="E6" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="83" t="s">
+      <c r="H6" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="82"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="33">
@@ -1441,12 +1505,12 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="71" t="s">
+      <c r="H8" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="77"/>
     </row>
     <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33">
@@ -1467,12 +1531,12 @@
       <c r="G9" s="1">
         <v>22</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="10" spans="2:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="33">
@@ -1493,12 +1557,12 @@
       <c r="G10" s="1">
         <v>32</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="80"/>
     </row>
     <row r="11" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="33">
@@ -1519,26 +1583,38 @@
       <c r="G11" s="1">
         <v>37</v>
       </c>
-      <c r="H11" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79"/>
+      <c r="H11" s="81" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
     </row>
     <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="33">
         <v>5</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="73"/>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>48</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="93"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="33">
@@ -1549,10 +1625,10 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="73"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="77"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="33">
@@ -1563,10 +1639,10 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="73"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="77"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="33">
@@ -1577,10 +1653,10 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="76"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="87"/>
     </row>
     <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="33">
@@ -1591,10 +1667,10 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="76"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="87"/>
     </row>
     <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="33">
@@ -1619,10 +1695,10 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="73"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="77"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
@@ -1647,13 +1723,13 @@
       <c r="G19" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="70"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="85"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -1702,6 +1778,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1710,19 +1797,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1734,7 +1810,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2274,14 +2350,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>11</v>
       </c>
       <c r="B12" s="25">
         <v>4</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D12" s="16" t="s">
         <v>80</v>
       </c>
@@ -2297,8 +2375,12 @@
       <c r="H12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="25"/>
+      <c r="I12" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="25">
+        <v>1</v>
+      </c>
       <c r="K12" s="16" t="s">
         <v>37</v>
       </c>
@@ -2308,17 +2390,21 @@
       <c r="M12" s="25">
         <v>35</v>
       </c>
-      <c r="N12" s="16"/>
+      <c r="N12" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:16" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="43">
         <v>12</v>
       </c>
       <c r="B13" s="25">
         <v>4</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D13" s="16" t="s">
         <v>80</v>
       </c>
@@ -2328,14 +2414,18 @@
       <c r="F13" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="66" t="s">
-        <v>85</v>
+      <c r="G13" s="90" t="s">
+        <v>76</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="44"/>
-      <c r="J13" s="25"/>
+      <c r="I13" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="25">
+        <v>1</v>
+      </c>
       <c r="K13" s="16" t="s">
         <v>37</v>
       </c>
@@ -2345,8 +2435,12 @@
       <c r="M13" s="25">
         <v>36</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
+      <c r="N13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:16" s="19" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43">
@@ -2355,7 +2449,9 @@
       <c r="B14" s="25">
         <v>4</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D14" s="20" t="s">
         <v>80</v>
       </c>
@@ -2363,16 +2459,20 @@
         <v>83</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="66" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>76</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="18"/>
+      <c r="I14" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="25">
+        <v>1</v>
+      </c>
       <c r="K14" s="20" t="s">
         <v>37</v>
       </c>
@@ -2382,46 +2482,98 @@
       <c r="M14" s="18">
         <v>37</v>
       </c>
-      <c r="N14" s="16"/>
-      <c r="O14" s="20"/>
-    </row>
-    <row r="15" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="N14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43">
         <v>14</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="25">
+        <v>5</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="89" t="s">
+        <v>93</v>
+      </c>
       <c r="J15" s="25"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="K15" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="25">
+        <v>1</v>
+      </c>
+      <c r="M15" s="25">
+        <v>38</v>
+      </c>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="43">
         <v>15</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
+      <c r="B16" s="25">
+        <v>5</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="25">
+        <v>10</v>
+      </c>
+      <c r="M16" s="25">
+        <v>48</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
@@ -3089,7 +3241,7 @@
       <c r="O51" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
iter 5 test cases
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37401DF-CCB8-4837-8BF9-5CC8C71656BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DED086-C22B-48F6-849B-4C617078E44D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="117">
   <si>
     <t>BUG METRICS</t>
   </si>
@@ -314,9 +314,6 @@
     <t>Did not change the method name when we renamed it in the DAO</t>
   </si>
   <si>
-    <t>31/08/2019</t>
-  </si>
-  <si>
     <t>Critical</t>
   </si>
   <si>
@@ -327,6 +324,54 @@
   </si>
   <si>
     <t>The bugs were discovered during the testing of the functionalities and hence we fixed it immediately upon discovery</t>
+  </si>
+  <si>
+    <t>Create Branch</t>
+  </si>
+  <si>
+    <t>Could not create branch record when you enter a phone number which starts with 6</t>
+  </si>
+  <si>
+    <t>Wrong validation for the phone number field</t>
+  </si>
+  <si>
+    <t>Edited the validation of the phone number to include numbers starting with 6</t>
+  </si>
+  <si>
+    <t>Delete Tutor</t>
+  </si>
+  <si>
+    <t>Delete Student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status Message displayed is "Failure! Something went wrong" when the delete was successful </t>
+  </si>
+  <si>
+    <t>Could not delete user successfully</t>
+  </si>
+  <si>
+    <t>Column name for SQL was wrong for deleteUser method</t>
+  </si>
+  <si>
+    <t>No error message displayed for failure of reset password</t>
+  </si>
+  <si>
+    <t>2efdaecb3eb4f2c981cb10fc39ad889836a46415</t>
+  </si>
+  <si>
+    <t>98f81d0849de43abd3076149e48edd5085463784</t>
+  </si>
+  <si>
+    <t>Create Grade</t>
+  </si>
+  <si>
+    <t>The tutor should not be able to create a grade record for the student when the grade field is empty</t>
+  </si>
+  <si>
+    <t>Did not validate for empty field</t>
+  </si>
+  <si>
+    <t>Add in validation for empty grade field</t>
   </si>
 </sst>
 </file>
@@ -336,11 +381,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -699,9 +751,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,10 +762,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,30 +776,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -765,40 +814,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,170 +856,167 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1398,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="126" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:K12"/>
+    <sheetView topLeftCell="A10" zoomScale="126" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1411,83 +1457,83 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="71" t="s">
+      <c r="H6" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="70"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>1</v>
       </c>
       <c r="C8" s="1">
@@ -1505,15 +1551,15 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="77"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="58"/>
     </row>
     <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>2</v>
       </c>
       <c r="C9" s="1">
@@ -1531,15 +1577,15 @@
       <c r="G9" s="1">
         <v>22</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="80"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="64"/>
     </row>
     <row r="10" spans="2:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <v>3</v>
       </c>
       <c r="C10" s="1">
@@ -1557,15 +1603,15 @@
       <c r="G10" s="1">
         <v>32</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="80"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="64"/>
     </row>
     <row r="11" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>4</v>
       </c>
       <c r="C11" s="1">
@@ -1583,22 +1629,22 @@
       <c r="G11" s="1">
         <v>37</v>
       </c>
-      <c r="H11" s="81" t="s">
+      <c r="H11" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1607,17 +1653,17 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>48</v>
-      </c>
-      <c r="H12" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="93"/>
+        <v>52</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>6</v>
       </c>
       <c r="C13" s="1"/>
@@ -1625,13 +1671,13 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="77"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="58"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>7</v>
       </c>
       <c r="C14" s="1"/>
@@ -1639,13 +1685,13 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="77"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="58"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="33">
+      <c r="B15" s="32">
         <v>8</v>
       </c>
       <c r="C15" s="1"/>
@@ -1653,13 +1699,13 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="87"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="61"/>
     </row>
     <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="33">
+      <c r="B16" s="32">
         <v>9</v>
       </c>
       <c r="C16" s="1"/>
@@ -1667,13 +1713,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="87"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="61"/>
     </row>
     <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>10</v>
       </c>
       <c r="C17" s="1"/>
@@ -1681,13 +1727,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>11</v>
       </c>
       <c r="C18" s="1"/>
@@ -1695,13 +1741,13 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="77"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="58"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="1">
@@ -1723,13 +1769,13 @@
       <c r="G19" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="85"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -1778,17 +1824,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1797,8 +1832,19 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -1807,17 +1853,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" style="20" customWidth="1"/>
     <col min="4" max="4" width="22.54296875" style="11" customWidth="1"/>
     <col min="5" max="5" width="48" style="13" customWidth="1"/>
     <col min="6" max="6" width="65.1796875" style="11" customWidth="1"/>
@@ -1833,1415 +1879,1560 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="30" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39">
+    <row r="2" spans="1:16" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="17">
         <v>2</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="17">
         <v>1</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="17">
         <v>5</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="17">
         <v>5</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="19" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39">
+    <row r="3" spans="1:16" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="38">
         <v>2</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="17">
         <v>0.2</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="17">
         <v>1</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>6</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="19" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39">
+    <row r="4" spans="1:16" s="18" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="38">
         <v>3</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="45">
         <v>0.5</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="17">
         <v>5</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <v>11</v>
       </c>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="42" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="39">
+    <row r="5" spans="1:16" s="40" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="38">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>2</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <v>0.2</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="17">
         <v>1</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <v>12</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="19" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39">
+    <row r="6" spans="1:16" s="18" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="38">
         <v>5</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>2</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>1.5</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="17">
         <v>5</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <v>17</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="19" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39">
+    <row r="7" spans="1:16" s="18" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="38">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="47">
         <v>43300</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="50">
+      <c r="I7" s="47">
         <v>43300</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="17">
         <v>1</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="17">
         <v>5</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <v>22</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="43">
+      <c r="A8" s="38">
         <v>7</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="17">
         <v>3</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="50">
+      <c r="G8" s="47">
         <v>43310</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="50">
+      <c r="I8" s="47">
         <v>43314</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>0.5</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <v>5</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>27</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="58" t="s">
+      <c r="O8" s="50" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="43">
+      <c r="A9" s="38">
         <v>8</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="17">
         <v>3</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="50">
+      <c r="G9" s="47">
         <v>43308</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="50">
+      <c r="I9" s="47">
         <v>43308</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="17">
         <v>0.5</v>
       </c>
-      <c r="K9" s="61" t="s">
+      <c r="K9" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="17">
         <v>5</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="17">
         <v>32</v>
       </c>
-      <c r="N9" s="61" t="s">
+      <c r="N9" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="61" t="s">
+      <c r="O9" s="79" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="43">
+      <c r="A10" s="38">
         <v>9</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="17">
         <v>4</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="81">
         <v>43325</v>
       </c>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="53">
+      <c r="I10" s="81">
         <v>43325</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="17">
         <v>0.2</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="17">
         <v>1</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="17">
         <v>33</v>
       </c>
-      <c r="N10" s="64" t="s">
+      <c r="N10" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="64" t="s">
+      <c r="O10" s="82" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="43">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="17">
         <v>4</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="81">
         <v>43325</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="65" t="s">
+      <c r="I11" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="17">
         <v>1</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="17">
         <v>1</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="17">
         <v>34</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="N11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="38">
         <v>11</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="17">
         <v>4</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="88" t="s">
+      <c r="I12" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="17">
         <v>1</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="17">
         <v>1</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="17">
         <v>35</v>
       </c>
-      <c r="N12" s="16" t="s">
+      <c r="N12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="16"/>
+      <c r="O12" s="19"/>
     </row>
     <row r="13" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="43">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="17">
         <v>4</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="90" t="s">
+      <c r="G13" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="88" t="s">
+      <c r="I13" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="17">
         <v>1</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="17">
         <v>1</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="17">
         <v>36</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="N13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="16" t="s">
+      <c r="O13" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="19" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43">
+    <row r="14" spans="1:16" s="18" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="38">
         <v>13</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="17">
         <v>4</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="90" t="s">
+      <c r="G14" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="88" t="s">
+      <c r="I14" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="17">
         <v>1</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <v>1</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="17">
         <v>37</v>
       </c>
-      <c r="N14" s="16" t="s">
+      <c r="N14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="43">
+      <c r="A15" s="38">
         <v>14</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="17">
         <v>5</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="89" t="s">
+      <c r="G15" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="20" t="s">
+      <c r="J15" s="17"/>
+      <c r="K15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="17">
         <v>1</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="17">
         <v>38</v>
       </c>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-    </row>
-    <row r="16" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="43">
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+    </row>
+    <row r="16" spans="1:16" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="38">
         <v>15</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="17">
         <v>5</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="89" t="s">
+      <c r="G16" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="L16" s="17">
+        <v>10</v>
+      </c>
+      <c r="M16" s="17">
+        <v>48</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="38">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17">
+        <v>5</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="89" t="s">
+      <c r="I17" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J17" s="17">
         <v>0.1</v>
       </c>
-      <c r="K16" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="L16" s="25">
-        <v>10</v>
-      </c>
-      <c r="M16" s="25">
-        <v>48</v>
-      </c>
-      <c r="N16" s="16" t="s">
+      <c r="K17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="17">
+        <v>1</v>
+      </c>
+      <c r="M17" s="17">
+        <v>49</v>
+      </c>
+      <c r="N17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="43">
-        <v>16</v>
-      </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43">
+      <c r="O17" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="38">
         <v>17</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-    </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="43">
+      <c r="B18" s="17">
+        <v>5</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="17">
+        <v>1</v>
+      </c>
+      <c r="M18" s="17">
+        <v>50</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="38">
         <v>18</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-    </row>
-    <row r="20" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="43">
+      <c r="B19" s="17">
+        <v>5</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="90" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="17">
+        <v>1</v>
+      </c>
+      <c r="M19" s="17">
+        <v>51</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="38"/>
+      <c r="B20" s="17">
+        <v>5</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="17">
+        <v>1</v>
+      </c>
+      <c r="M20" s="17">
+        <v>52</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="38">
         <v>19</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-    </row>
-    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="43">
+      <c r="B21" s="17">
+        <v>6</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="90" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="51">
+        <v>43382</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="39"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" s="17">
+        <v>5</v>
+      </c>
+      <c r="M21" s="17">
+        <v>56</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+    </row>
+    <row r="22" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="41">
         <v>20</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-    </row>
-    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="43">
-        <v>21</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="25"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="43">
-        <v>22</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="16"/>
+    <row r="23" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="41">
+        <v>21</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="25"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="24"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="43">
-        <v>23</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="41">
+        <v>22</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="25"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="24"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="43">
-        <v>24</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="41">
+        <v>23</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="25"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="24"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="43">
-        <v>25</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="41">
+        <v>24</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="25"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="43">
-        <v>26</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="41">
+        <v>25</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="25"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="24"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="43">
-        <v>27</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="20"/>
+      <c r="A28" s="41">
+        <v>26</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="25"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="24"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="43">
+      <c r="A29" s="41">
+        <v>27</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="41">
         <v>28</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-    </row>
-    <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="43">
+      <c r="B30" s="24"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+    </row>
+    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="41">
         <v>29</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-    </row>
-    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="43">
+      <c r="B31" s="24"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="41">
         <v>30</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-    </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="43">
-        <v>31</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="44"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
     </row>
-    <row r="33" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="43">
-        <v>32</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="20"/>
+    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="41">
+        <v>31</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="44"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="43">
-        <v>33</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="41">
+        <v>32</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="44"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="24"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="43">
-        <v>34</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="20"/>
+      <c r="A35" s="41">
+        <v>33</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="44"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="16"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="24"/>
       <c r="K35" s="16"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
     </row>
     <row r="36" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="43">
-        <v>35</v>
-      </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="41">
+        <v>34</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="44"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="16"/>
       <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="J36" s="24"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
     </row>
     <row r="37" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="43">
-        <v>36</v>
-      </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="41">
+        <v>35</v>
+      </c>
+      <c r="B37" s="24"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="44"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="16"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
       <c r="K37" s="16"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
     </row>
     <row r="38" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="43">
-        <v>37</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="41">
+        <v>36</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="44"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="16"/>
       <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
+      <c r="J38" s="24"/>
       <c r="K38" s="16"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
     </row>
     <row r="39" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="43">
-        <v>38</v>
-      </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="20"/>
+      <c r="A39" s="41">
+        <v>37</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="44"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="16"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
       <c r="K39" s="16"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
     </row>
     <row r="40" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="43">
-        <v>39</v>
-      </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="20"/>
+      <c r="A40" s="41">
+        <v>38</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="44"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="16"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="24"/>
       <c r="K40" s="16"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
     </row>
     <row r="41" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="43">
-        <v>40</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="20"/>
+      <c r="A41" s="41">
+        <v>39</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="44"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="16"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="24"/>
       <c r="K41" s="16"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
     </row>
     <row r="42" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="43">
-        <v>41</v>
-      </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="20"/>
+      <c r="A42" s="41">
+        <v>40</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="26"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="16"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="24"/>
       <c r="K42" s="16"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
     </row>
     <row r="43" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="41">
+        <v>41</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="26"/>
+      <c r="G43" s="25"/>
       <c r="H43" s="16"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="24"/>
       <c r="K43" s="16"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
       <c r="N43" s="16"/>
       <c r="O43" s="16"/>
     </row>
     <row r="44" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="43">
-        <v>43</v>
-      </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="41">
+        <v>42</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="44"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="24"/>
       <c r="K44" s="16"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="43">
-        <v>44</v>
-      </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="41">
+        <v>43</v>
+      </c>
+      <c r="B45" s="24"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="44"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="16"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="24"/>
       <c r="K45" s="16"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
     <row r="46" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="43">
-        <v>45</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="41">
+        <v>44</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="44"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="16"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="24"/>
       <c r="K46" s="16"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
     </row>
     <row r="47" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="43">
-        <v>46</v>
-      </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="20"/>
+      <c r="A47" s="41">
+        <v>45</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
-      <c r="G47" s="44"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="24"/>
       <c r="K47" s="16"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
     </row>
     <row r="48" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="43">
-        <v>47</v>
-      </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="45"/>
+      <c r="A48" s="41">
+        <v>46</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="44"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="16"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="24"/>
       <c r="K48" s="16"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
     </row>
     <row r="49" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="43">
-        <v>48</v>
-      </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="20"/>
+      <c r="A49" s="41">
+        <v>47</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="43"/>
       <c r="D49" s="16"/>
-      <c r="E49" s="37"/>
+      <c r="E49" s="16"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="44"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="16"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="24"/>
       <c r="K49" s="16"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
     </row>
     <row r="50" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="43">
-        <v>49</v>
-      </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="41">
+        <v>48</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
+      <c r="E50" s="36"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="44"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="16"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="24"/>
       <c r="K50" s="16"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
     </row>
     <row r="51" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="43">
+      <c r="A51" s="41">
+        <v>49</v>
+      </c>
+      <c r="B51" s="24"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="41">
         <v>50</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="37"/>
-      <c r="O51" s="16"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated bug metrics and wiki template
</commit_message>
<xml_diff>
--- a/metrics/Team eXi Bug Metrics.xlsx
+++ b/metrics/Team eXi Bug Metrics.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHMOHSAN\Desktop\Thriving-Stones-Project\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xin\Documents\FYP\Thriving-Stones-Project\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2BFE26E-0DB3-4B59-AD95-1241E6DA0B38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0994CDA-F35E-4037-BAFB-8511E32C9A29}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25760" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1314,6 +1321,60 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1324,15 +1385,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1340,51 +1392,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1812,11 +1819,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:K14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="13.54296875" customWidth="1"/>
     <col min="4" max="4" width="16.54296875" customWidth="1"/>
@@ -1824,83 +1831,83 @@
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B3" s="88" t="s">
+    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.75">
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.75">
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.75">
-      <c r="B6" s="89" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="93" t="s">
+      <c r="E6" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="93" t="s">
+      <c r="F6" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.75">
-      <c r="B7" s="90"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="75"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="29">
         <v>1</v>
       </c>
@@ -1919,14 +1926,14 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="80" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="81"/>
       <c r="J8" s="81"/>
       <c r="K8" s="82"/>
     </row>
-    <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="29">
         <v>2</v>
       </c>
@@ -1945,14 +1952,14 @@
       <c r="G9" s="1">
         <v>22</v>
       </c>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="86"/>
-    </row>
-    <row r="10" spans="2:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="85"/>
+    </row>
+    <row r="10" spans="2:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="29">
         <v>3</v>
       </c>
@@ -1971,14 +1978,14 @@
       <c r="G10" s="1">
         <v>32</v>
       </c>
-      <c r="H10" s="84" t="s">
+      <c r="H10" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="86"/>
-    </row>
-    <row r="11" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="85"/>
+    </row>
+    <row r="11" spans="2:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="29">
         <v>4</v>
       </c>
@@ -1997,14 +2004,14 @@
       <c r="G11" s="1">
         <v>37</v>
       </c>
-      <c r="H11" s="87" t="s">
+      <c r="H11" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="86"/>
-    </row>
-    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="85"/>
+    </row>
+    <row r="12" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="29">
         <v>5</v>
       </c>
@@ -2023,14 +2030,14 @@
       <c r="G12" s="1">
         <v>52</v>
       </c>
-      <c r="H12" s="75" t="s">
+      <c r="H12" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="2:11" ht="56" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="89"/>
+    </row>
+    <row r="13" spans="2:11" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="29">
         <v>6</v>
       </c>
@@ -2049,14 +2056,14 @@
       <c r="G13" s="1">
         <v>66</v>
       </c>
-      <c r="H13" s="75" t="s">
+      <c r="H13" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="77"/>
-    </row>
-    <row r="14" spans="2:11" ht="52" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="89"/>
+    </row>
+    <row r="14" spans="2:11" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="29">
         <v>7</v>
       </c>
@@ -2064,10 +2071,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
         <v>5</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
@@ -2075,14 +2082,14 @@
       <c r="G14" s="1">
         <v>124</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="H14" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="77"/>
-    </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="89"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="29">
         <v>8</v>
       </c>
@@ -2091,12 +2098,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="80"/>
-    </row>
-    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="H15" s="93"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="95"/>
+    </row>
+    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="29">
         <v>9</v>
       </c>
@@ -2105,12 +2112,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="80"/>
-    </row>
-    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="H16" s="93"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="95"/>
+    </row>
+    <row r="17" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="29">
         <v>10</v>
       </c>
@@ -2124,7 +2131,7 @@
       <c r="J17" s="21"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="29">
         <v>11</v>
       </c>
@@ -2133,12 +2140,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="78"/>
+      <c r="H18" s="93"/>
       <c r="I18" s="81"/>
       <c r="J18" s="81"/>
       <c r="K18" s="82"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="29" t="s">
         <v>8</v>
       </c>
@@ -2148,11 +2155,11 @@
       </c>
       <c r="D19" s="1">
         <f>SUM(D13:D18)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1">
         <f>SUM(E13:E18)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19" s="1">
         <f>SUM(F13:F18)</f>
@@ -2160,16 +2167,16 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B21" s="72" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B21" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="74"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="92"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -2178,7 +2185,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2187,7 +2194,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2196,7 +2203,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2205,7 +2212,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -2216,6 +2223,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B3:K5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -2224,17 +2242,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2247,11 +2254,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CV54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView topLeftCell="D30" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="12" customWidth="1"/>
     <col min="2" max="2" width="8.81640625" style="23" customWidth="1"/>
@@ -2270,7 +2277,7 @@
     <col min="17" max="16384" width="8.81640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
@@ -2318,7 +2325,7 @@
       </c>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:100" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:100" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -2620,7 +2627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:100" s="17" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:100" s="17" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="34">
         <v>2</v>
       </c>
@@ -2667,7 +2674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:100" s="17" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:100" s="17" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34">
         <v>3</v>
       </c>
@@ -2714,7 +2721,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:100" s="36" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:100" s="36" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="34">
         <v>4</v>
       </c>
@@ -2761,7 +2768,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:100" s="17" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:100" s="17" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="34">
         <v>5</v>
       </c>
@@ -2808,7 +2815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:100" s="17" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:100" s="17" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34">
         <v>6</v>
       </c>
@@ -2855,7 +2862,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="34">
         <v>7</v>
       </c>
@@ -2902,7 +2909,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:100" ht="59" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -2949,7 +2956,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="34">
         <v>9</v>
       </c>
@@ -2996,7 +3003,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -3043,7 +3050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="34">
         <v>11</v>
       </c>
@@ -3088,7 +3095,7 @@
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:100" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="34">
         <v>12</v>
       </c>
@@ -3135,7 +3142,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:100" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:100" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -3182,7 +3189,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:100" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:100" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="34">
         <v>14</v>
       </c>
@@ -3221,7 +3228,7 @@
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:100" ht="45.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:100" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34">
         <v>15</v>
       </c>
@@ -3268,7 +3275,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="50.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34">
         <v>16</v>
       </c>
@@ -3315,7 +3322,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34">
         <v>17</v>
       </c>
@@ -3362,7 +3369,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="34">
         <v>18</v>
       </c>
@@ -3409,7 +3416,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="34"/>
       <c r="B20" s="16">
         <v>5</v>
@@ -3454,7 +3461,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="34">
         <v>19</v>
       </c>
@@ -3501,7 +3508,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="34">
         <v>20</v>
       </c>
@@ -3548,7 +3555,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34">
         <v>21</v>
       </c>
@@ -3591,7 +3598,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="34">
         <v>22</v>
       </c>
@@ -3638,7 +3645,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="34">
         <v>23</v>
       </c>
@@ -3685,7 +3692,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="41" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:15" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="34">
         <v>24</v>
       </c>
@@ -3732,7 +3739,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="41" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:15" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34">
         <v>25</v>
       </c>
@@ -3779,7 +3786,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="34">
         <v>26</v>
       </c>
@@ -3826,7 +3833,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="34">
         <v>27</v>
       </c>
@@ -3873,7 +3880,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="34">
         <v>28</v>
       </c>
@@ -3920,7 +3927,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="34">
         <v>29</v>
       </c>
@@ -3967,7 +3974,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="34">
         <v>30</v>
       </c>
@@ -4014,7 +4021,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="62.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:15" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="34">
         <v>31</v>
       </c>
@@ -4061,7 +4068,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="34">
         <v>32</v>
       </c>
@@ -4096,7 +4103,7 @@
       <c r="N34" s="18"/>
       <c r="O34" s="18"/>
     </row>
-    <row r="35" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="34">
         <v>33</v>
       </c>
@@ -4131,7 +4138,7 @@
       <c r="N35" s="18"/>
       <c r="O35" s="18"/>
     </row>
-    <row r="36" spans="1:15" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A36" s="34">
         <v>34</v>
       </c>
@@ -4168,7 +4175,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="34">
         <v>35</v>
       </c>
@@ -4207,7 +4214,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="34">
         <v>36</v>
       </c>
@@ -4244,7 +4251,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="34">
         <v>37</v>
       </c>
@@ -4275,7 +4282,7 @@
       <c r="N39" s="67"/>
       <c r="O39" s="67"/>
     </row>
-    <row r="40" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="34">
         <v>38</v>
       </c>
@@ -4306,7 +4313,7 @@
       <c r="N40" s="67"/>
       <c r="O40" s="67"/>
     </row>
-    <row r="41" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="34">
         <v>39</v>
       </c>
@@ -4353,7 +4360,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="34">
         <v>40</v>
       </c>
@@ -4400,7 +4407,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="59" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="34">
         <v>41</v>
       </c>
@@ -4447,7 +4454,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="34">
         <v>42</v>
       </c>
@@ -4478,7 +4485,7 @@
       <c r="J44" s="16">
         <v>5</v>
       </c>
-      <c r="K44" s="95" t="s">
+      <c r="K44" s="72" t="s">
         <v>30</v>
       </c>
       <c r="L44" s="16">
@@ -4487,14 +4494,14 @@
       <c r="M44" s="16">
         <v>142</v>
       </c>
-      <c r="N44" s="95" t="s">
+      <c r="N44" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="O44" s="95" t="s">
+      <c r="O44" s="72" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="34">
         <v>43</v>
       </c>
@@ -4504,13 +4511,13 @@
       <c r="C45" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="D45" s="95" t="s">
+      <c r="D45" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="E45" s="95" t="s">
+      <c r="E45" s="72" t="s">
         <v>217</v>
       </c>
-      <c r="F45" s="95" t="s">
+      <c r="F45" s="72" t="s">
         <v>218</v>
       </c>
       <c r="G45" s="62">
@@ -4525,7 +4532,7 @@
       <c r="J45" s="16">
         <v>5</v>
       </c>
-      <c r="K45" s="95" t="s">
+      <c r="K45" s="72" t="s">
         <v>30</v>
       </c>
       <c r="L45" s="16">
@@ -4534,14 +4541,14 @@
       <c r="M45" s="16">
         <v>147</v>
       </c>
-      <c r="N45" s="95" t="s">
+      <c r="N45" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="O45" s="95" t="s">
+      <c r="O45" s="72" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="34">
         <v>44</v>
       </c>
@@ -4564,7 +4571,7 @@
       <c r="N46" s="18"/>
       <c r="O46" s="18"/>
     </row>
-    <row r="47" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="34">
         <v>45</v>
       </c>
@@ -4573,7 +4580,7 @@
       <c r="D47" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="E47" s="95" t="s">
+      <c r="E47" s="72" t="s">
         <v>221</v>
       </c>
       <c r="F47" s="18"/>
@@ -4587,7 +4594,7 @@
       <c r="N47" s="18"/>
       <c r="O47" s="18"/>
     </row>
-    <row r="48" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="34">
         <v>46</v>
       </c>
@@ -4596,7 +4603,7 @@
       <c r="D48" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="E48" s="95" t="s">
+      <c r="E48" s="72" t="s">
         <v>220</v>
       </c>
       <c r="F48" s="18"/>
@@ -4610,7 +4617,7 @@
       <c r="N48" s="18"/>
       <c r="O48" s="18"/>
     </row>
-    <row r="49" spans="1:15" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="34">
         <v>47</v>
       </c>
@@ -4619,7 +4626,7 @@
       <c r="D49" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="95" t="s">
+      <c r="E49" s="72" t="s">
         <v>222</v>
       </c>
       <c r="F49" s="18"/>
@@ -4633,7 +4640,7 @@
       <c r="N49" s="18"/>
       <c r="O49" s="18"/>
     </row>
-    <row r="50" spans="1:15" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="34">
         <v>48</v>
       </c>
@@ -4652,7 +4659,7 @@
       <c r="N50" s="18"/>
       <c r="O50" s="18"/>
     </row>
-    <row r="51" spans="1:15" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="34">
         <v>49</v>
       </c>
@@ -4671,7 +4678,7 @@
       <c r="N51" s="18"/>
       <c r="O51" s="18"/>
     </row>
-    <row r="52" spans="1:15" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="34">
         <v>50</v>
       </c>
@@ -4690,7 +4697,7 @@
       <c r="N52" s="64"/>
       <c r="O52" s="18"/>
     </row>
-    <row r="54" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C54" s="11"/>
       <c r="D54" s="15"/>
       <c r="E54" s="11"/>

</xml_diff>